<commit_message>
added project pictures and some css
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahen\Desktop\Personal Projects\personal-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E926F4F-A22D-4CA2-B846-36D15231306D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5848D22-1072-42B1-9DE4-0D73E0490E0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="140" windowWidth="14400" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Hours</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>6:30pm</t>
+  </si>
+  <si>
+    <t>7:45pm</t>
+  </si>
+  <si>
+    <t>7:44pm</t>
+  </si>
+  <si>
+    <t>10:25pm</t>
   </si>
 </sst>
 </file>
@@ -355,10 +364,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -384,8 +393,28 @@
       <c r="A2" s="1">
         <v>43827</v>
       </c>
+      <c r="B2">
+        <v>1.25</v>
+      </c>
       <c r="C2" t="s">
         <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>43828</v>
+      </c>
+      <c r="B3">
+        <v>2.5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added icons, bootstrap and more css
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahen\Desktop\Personal Projects\personal-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5848D22-1072-42B1-9DE4-0D73E0490E0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DBE07D-F5D2-4DB0-BB9A-44C2D0A8A165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="140" windowWidth="14400" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Hours</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>10:25pm</t>
+  </si>
+  <si>
+    <t>1pm</t>
+  </si>
+  <si>
+    <t>3pm</t>
   </si>
 </sst>
 </file>
@@ -364,10 +370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -417,6 +423,17 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>43829</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed some contents and some css, and added pictures I might want to use
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahen\Desktop\Personal Projects\personal-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DBE07D-F5D2-4DB0-BB9A-44C2D0A8A165}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614CAA32-AF4D-4C83-9D05-051BA277A0A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="140" windowWidth="14400" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Hours</t>
   </si>
@@ -52,6 +52,12 @@
   </si>
   <si>
     <t>3pm</t>
+  </si>
+  <si>
+    <t>6:45pm</t>
+  </si>
+  <si>
+    <t>10pm</t>
   </si>
 </sst>
 </file>
@@ -370,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -427,11 +433,25 @@
       <c r="A4" s="1">
         <v>43829</v>
       </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>3.25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed "about me" layout, and added a welcome section
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahen\Desktop\Personal Projects\personal-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614CAA32-AF4D-4C83-9D05-051BA277A0A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAECDA8-8B81-41B2-A933-A2E9BDE6C00D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="140" windowWidth="14400" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Hours</t>
   </si>
@@ -58,6 +58,12 @@
   </si>
   <si>
     <t>10pm</t>
+  </si>
+  <si>
+    <t>11pm</t>
+  </si>
+  <si>
+    <t>12:30pm</t>
   </si>
 </sst>
 </file>
@@ -376,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -454,6 +460,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>1.5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
changed the transition section, and improved css styles
I decided on a quote for the transition section, then chose fonts and colors to use, customized my buttons, and modified some paddings and margins.
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahen\Desktop\Personal Projects\personal-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BAECDA8-8B81-41B2-A933-A2E9BDE6C00D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8075106-CFC7-4C5F-8448-7BECF3276A91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="140" windowWidth="14400" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Hours</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>12:30pm</t>
+  </si>
+  <si>
+    <t>7pm</t>
+  </si>
+  <si>
+    <t>10:30pm</t>
   </si>
 </sst>
 </file>
@@ -382,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -471,6 +477,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>43857</v>
+      </c>
+      <c r="B7">
+        <v>3.5</v>
+      </c>
+      <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Populated the Projects section and improved css styles
</commit_message>
<xml_diff>
--- a/Timesheet.xlsx
+++ b/Timesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahen\Desktop\Personal Projects\personal-website\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8075106-CFC7-4C5F-8448-7BECF3276A91}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8633AF44-33F7-4CF3-8CF8-C01368A75F69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="140" windowWidth="14400" windowHeight="10200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Hours</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>10:30pm</t>
+  </si>
+  <si>
+    <t>11:54pm</t>
+  </si>
+  <si>
+    <t>1:45am</t>
+  </si>
+  <si>
+    <t>3:45am</t>
   </si>
 </sst>
 </file>
@@ -388,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -491,6 +500,31 @@
         <v>14</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>43858</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>